<commit_message>
Update dashboard logic and contractor mapping
</commit_message>
<xml_diff>
--- a/Contractor File.xlsx
+++ b/Contractor File.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usps365-my.sharepoint.com/personal/casey_y_smith_usps_gov/Documents/Test Folder/versionone-dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{D8D9F938-1052-41E2-8A93-A3B409169C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CB10608-BDEE-499D-9D20-84ED9D0BD4DB}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{D8D9F938-1052-41E2-8A93-A3B409169C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF0B3033-DE22-47A4-AAD8-8DD21B8D4502}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{19EB4502-440B-4CBA-8D4E-972E96BDBE67}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{19EB4502-440B-4CBA-8D4E-972E96BDBE67}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,24 +44,6 @@
     <t>Names</t>
   </si>
   <si>
-    <t>CDAS 6441</t>
-  </si>
-  <si>
-    <t>EDS 4834</t>
-  </si>
-  <si>
-    <t>EEB 9372</t>
-  </si>
-  <si>
-    <t>UAP SPM 9442</t>
-  </si>
-  <si>
-    <t>UAP IV 9443</t>
-  </si>
-  <si>
-    <t>SAL 9402</t>
-  </si>
-  <si>
     <t>ACCENTURE</t>
   </si>
   <si>
@@ -561,6 +543,24 @@
   </si>
   <si>
     <t>Will Sheehan</t>
+  </si>
+  <si>
+    <t>CDAS-6441</t>
+  </si>
+  <si>
+    <t>EDS-4834</t>
+  </si>
+  <si>
+    <t>EEB-9372</t>
+  </si>
+  <si>
+    <t>UAP-SPM-9442</t>
+  </si>
+  <si>
+    <t>UAP-IV-9443</t>
+  </si>
+  <si>
+    <t>UAPSAL-9402</t>
   </si>
 </sst>
 </file>
@@ -941,15 +941,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25211BDE-564C-47B6-9199-FF409C50DBD8}">
   <dimension ref="A1:I160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="B151" sqref="B151"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="9.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -961,30 +967,30 @@
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>169</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>170</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>171</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>172</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>173</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
@@ -1000,10 +1006,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1">
         <v>88</v>
@@ -1019,10 +1025,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1">
         <v>66</v>
@@ -1038,10 +1044,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1">
         <v>81</v>
@@ -1059,10 +1065,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1">
         <v>87</v>
@@ -1078,10 +1084,10 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="C7" s="1">
         <v>30.75</v>
@@ -1097,10 +1103,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1">
         <v>0</v>
@@ -1116,10 +1122,10 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C9" s="1">
         <v>62</v>
@@ -1135,10 +1141,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1">
         <v>0</v>
@@ -1154,10 +1160,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C11" s="1">
         <v>0</v>
@@ -1173,10 +1179,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1">
         <v>85</v>
@@ -1192,10 +1198,10 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C13" s="1">
         <v>0</v>
@@ -1211,10 +1217,10 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C14" s="1">
         <v>0</v>
@@ -1230,10 +1236,10 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C15" s="1">
         <v>85.25</v>
@@ -1249,10 +1255,10 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C16" s="1">
         <v>0</v>
@@ -1270,10 +1276,10 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C17" s="1">
         <v>32</v>
@@ -1289,10 +1295,10 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C18" s="1">
         <v>14</v>
@@ -1308,10 +1314,10 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C19" s="1">
         <v>0</v>
@@ -1327,10 +1333,10 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C20" s="1">
         <v>57</v>
@@ -1346,10 +1352,10 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C21" s="1">
         <v>65.25</v>
@@ -1365,10 +1371,10 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C22" s="1">
         <v>80</v>
@@ -1384,10 +1390,10 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C23" s="1">
         <v>0</v>
@@ -1403,10 +1409,10 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C24" s="1">
         <v>107.5</v>
@@ -1422,10 +1428,10 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C25" s="1">
         <v>0</v>
@@ -1441,10 +1447,10 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C26" s="1">
         <v>0</v>
@@ -1458,10 +1464,10 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C27" s="1">
         <v>65.5</v>
@@ -1477,10 +1483,10 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C28" s="1">
         <v>45.5</v>
@@ -1496,10 +1502,10 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C29" s="1">
         <v>0</v>
@@ -1515,10 +1521,10 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C30" s="1">
         <v>1</v>
@@ -1534,10 +1540,10 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C31" s="1">
         <v>80</v>
@@ -1555,10 +1561,10 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C32" s="1">
         <v>33.5</v>
@@ -1574,10 +1580,10 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C33" s="1">
         <v>0</v>
@@ -1595,10 +1601,10 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C34" s="1">
         <v>0</v>
@@ -1612,10 +1618,10 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C35" s="1">
         <v>45</v>
@@ -1633,10 +1639,10 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C36" s="1">
         <v>56</v>
@@ -1652,10 +1658,10 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C37" s="1">
         <v>0</v>
@@ -1671,10 +1677,10 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C38" s="1">
         <v>0</v>
@@ -1690,10 +1696,10 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C39" s="1">
         <v>16</v>
@@ -1709,10 +1715,10 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C40" s="1">
         <v>80</v>
@@ -1728,10 +1734,10 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C41" s="1">
         <v>80</v>
@@ -1755,10 +1761,10 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C42" s="1">
         <v>54</v>
@@ -1774,10 +1780,10 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C43" s="1">
         <v>16</v>
@@ -1795,10 +1801,10 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C44" s="1">
         <v>101</v>
@@ -1814,10 +1820,10 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C45" s="1">
         <v>0</v>
@@ -1833,10 +1839,10 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C46" s="1">
         <v>56</v>
@@ -1852,10 +1858,10 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C47" s="1">
         <v>0</v>
@@ -1871,10 +1877,10 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C48" s="1">
         <v>55</v>
@@ -1890,10 +1896,10 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C49" s="1">
         <v>70</v>
@@ -1909,10 +1915,10 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C50" s="1">
         <v>7</v>
@@ -1928,10 +1934,10 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C51" s="1">
         <v>78</v>
@@ -1947,10 +1953,10 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C52" s="1">
         <v>0</v>
@@ -1966,10 +1972,10 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C53" s="1">
         <v>236</v>
@@ -1985,10 +1991,10 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C54" s="1">
         <v>0</v>
@@ -2002,10 +2008,10 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C55" s="1">
         <v>33.5</v>
@@ -2023,10 +2029,10 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C56" s="1">
         <v>79</v>
@@ -2042,10 +2048,10 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C57" s="1">
         <v>87</v>
@@ -2061,10 +2067,10 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C58" s="1">
         <v>0</v>
@@ -2080,10 +2086,10 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C59" s="1">
         <v>23.5</v>
@@ -2099,10 +2105,10 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C60" s="1">
         <v>0</v>
@@ -2118,10 +2124,10 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C61" s="1">
         <v>64</v>
@@ -2137,10 +2143,10 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C62" s="1">
         <v>39</v>
@@ -2158,10 +2164,10 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C63" s="1">
         <v>86.75</v>
@@ -2177,10 +2183,10 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C64" s="1">
         <v>49</v>
@@ -2200,10 +2206,10 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C65" s="1">
         <v>0</v>
@@ -2217,10 +2223,10 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C66" s="1">
         <v>80</v>
@@ -2236,10 +2242,10 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C67" s="1">
         <v>72.5</v>
@@ -2255,10 +2261,10 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C68" s="1">
         <v>70</v>
@@ -2274,10 +2280,10 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C69" s="1">
         <v>82</v>
@@ -2295,10 +2301,10 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C70" s="1">
         <v>60</v>
@@ -2314,10 +2320,10 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C71" s="1">
         <v>0</v>
@@ -2333,10 +2339,10 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C72" s="1">
         <v>88</v>
@@ -2352,10 +2358,10 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C73" s="1">
         <v>1</v>
@@ -2371,10 +2377,10 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C74" s="1">
         <v>79</v>
@@ -2390,10 +2396,10 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C75" s="1">
         <v>0</v>
@@ -2407,10 +2413,10 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C76" s="1">
         <v>0</v>
@@ -2424,10 +2430,10 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C77" s="1">
         <v>8</v>
@@ -2443,10 +2449,10 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C78" s="1">
         <v>80</v>
@@ -2466,10 +2472,10 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C79" s="1">
         <v>80</v>
@@ -2485,10 +2491,10 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C80" s="1">
         <v>0</v>
@@ -2504,10 +2510,10 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C81" s="1">
         <v>0</v>
@@ -2523,10 +2529,10 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C82" s="1">
         <v>84.5</v>
@@ -2542,10 +2548,10 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C83" s="1">
         <v>87</v>
@@ -2561,10 +2567,10 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C84" s="1">
         <v>30</v>
@@ -2582,10 +2588,10 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C85" s="1">
         <v>63</v>
@@ -2601,10 +2607,10 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C86" s="1">
         <v>68</v>
@@ -2620,10 +2626,10 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C87" s="1">
         <v>54</v>
@@ -2639,10 +2645,10 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C88" s="1">
         <v>0</v>
@@ -2656,10 +2662,10 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C89" s="1">
         <v>81</v>
@@ -2675,10 +2681,10 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C90" s="1">
         <v>49</v>
@@ -2694,10 +2700,10 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C91" s="1">
         <v>0</v>
@@ -2711,10 +2717,10 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C92" s="1">
         <v>49</v>
@@ -2732,10 +2738,10 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C93" s="1">
         <v>0</v>
@@ -2751,10 +2757,10 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C94" s="1">
         <v>0</v>
@@ -2768,10 +2774,10 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C95" s="1">
         <v>0</v>
@@ -2787,10 +2793,10 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C96" s="1">
         <v>0</v>
@@ -2804,10 +2810,10 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C97" s="1">
         <v>0</v>
@@ -2823,10 +2829,10 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C98" s="1">
         <v>39</v>
@@ -2842,10 +2848,10 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C99" s="1">
         <v>80</v>
@@ -2863,10 +2869,10 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C100" s="1">
         <v>0</v>
@@ -2880,10 +2886,10 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C101" s="1">
         <v>56</v>
@@ -2899,10 +2905,10 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C102" s="1">
         <v>9</v>
@@ -2918,10 +2924,10 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C103" s="1">
         <v>87</v>
@@ -2937,10 +2943,10 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C104" s="1">
         <v>80</v>
@@ -2956,10 +2962,10 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C105" s="1">
         <v>80</v>
@@ -2975,10 +2981,10 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C106" s="1">
         <v>80</v>
@@ -2994,10 +3000,10 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C107" s="1">
         <v>96</v>
@@ -3013,10 +3019,10 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C108" s="1">
         <v>0</v>
@@ -3034,10 +3040,10 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C109" s="1">
         <v>9</v>
@@ -3053,10 +3059,10 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C110" s="1">
         <v>0</v>
@@ -3072,10 +3078,10 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C111" s="1">
         <v>40</v>
@@ -3091,10 +3097,10 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C112" s="1">
         <v>0</v>
@@ -3108,10 +3114,10 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C113" s="1">
         <v>36</v>
@@ -3127,10 +3133,10 @@
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C114" s="1">
         <v>0</v>
@@ -3146,10 +3152,10 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C115" s="1">
         <v>80</v>
@@ -3165,10 +3171,10 @@
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C116" s="1">
         <v>0</v>
@@ -3182,10 +3188,10 @@
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C117" s="1">
         <v>71</v>
@@ -3201,10 +3207,10 @@
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C118" s="1">
         <v>88</v>
@@ -3220,10 +3226,10 @@
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C119" s="1">
         <v>0</v>
@@ -3243,10 +3249,10 @@
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C120" s="1">
         <v>56</v>
@@ -3262,10 +3268,10 @@
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C121" s="1">
         <v>0</v>
@@ -3281,10 +3287,10 @@
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C122" s="1">
         <v>6.5</v>
@@ -3300,10 +3306,10 @@
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C123" s="1">
         <v>4.5</v>
@@ -3321,10 +3327,10 @@
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C124" s="1">
         <v>0</v>
@@ -3340,10 +3346,10 @@
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C125" s="1">
         <v>76</v>
@@ -3359,10 +3365,10 @@
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C126" s="1">
         <v>0</v>
@@ -3378,10 +3384,10 @@
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C127" s="1">
         <v>0</v>
@@ -3397,10 +3403,10 @@
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C128" s="1">
         <v>0</v>
@@ -3416,10 +3422,10 @@
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C129" s="1">
         <v>0</v>
@@ -3433,10 +3439,10 @@
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C130" s="1">
         <v>0</v>
@@ -3450,10 +3456,10 @@
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C131" s="1">
         <v>25</v>
@@ -3471,10 +3477,10 @@
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C132" s="1">
         <v>0</v>
@@ -3488,10 +3494,10 @@
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C133" s="1">
         <v>107</v>
@@ -3507,10 +3513,10 @@
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C134" s="1">
         <v>83</v>
@@ -3526,10 +3532,10 @@
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C135" s="1">
         <v>75</v>
@@ -3545,10 +3551,10 @@
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C136" s="1">
         <v>65</v>
@@ -3564,10 +3570,10 @@
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C137" s="1">
         <v>81</v>
@@ -3583,10 +3589,10 @@
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C138" s="1">
         <v>75</v>
@@ -3602,10 +3608,10 @@
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C139" s="1">
         <v>6</v>
@@ -3623,10 +3629,10 @@
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C140" s="1">
         <v>61</v>
@@ -3642,10 +3648,10 @@
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C141" s="1">
         <v>88</v>
@@ -3665,10 +3671,10 @@
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C142" s="1">
         <v>67</v>
@@ -3684,10 +3690,10 @@
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C143" s="1">
         <v>42</v>
@@ -3703,10 +3709,10 @@
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C144" s="1">
         <v>113.5</v>
@@ -3722,10 +3728,10 @@
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C145" s="1">
         <v>0</v>
@@ -3739,10 +3745,10 @@
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C146" s="1">
         <v>7</v>
@@ -3758,10 +3764,10 @@
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C147" s="1">
         <v>0</v>
@@ -3777,10 +3783,10 @@
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C148" s="1">
         <v>0</v>
@@ -3796,10 +3802,10 @@
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C149" s="1">
         <v>66</v>
@@ -3817,10 +3823,10 @@
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C150" s="1">
         <v>64</v>
@@ -3836,10 +3842,10 @@
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C151" s="1">
         <v>0</v>
@@ -3855,10 +3861,10 @@
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C152" s="1">
         <v>81</v>
@@ -3874,10 +3880,10 @@
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C153" s="1">
         <v>72</v>
@@ -3893,10 +3899,10 @@
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C154" s="1">
         <v>0</v>
@@ -3912,10 +3918,10 @@
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C155" s="1">
         <v>0</v>
@@ -3931,10 +3937,10 @@
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C156" s="1">
         <v>80</v>
@@ -3952,10 +3958,10 @@
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C157" s="1">
         <v>80</v>
@@ -3971,10 +3977,10 @@
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C158" s="1">
         <v>0</v>
@@ -3988,10 +3994,10 @@
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C159" s="1">
         <v>16</v>
@@ -4007,10 +4013,10 @@
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C160" s="1">
         <v>76</v>

</xml_diff>